<commit_message>
Completed function test descriptions and traceability matrix file
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms3-traceability-matrix-group5-1.xlsx
+++ b/Documents/Testing/TestsDocuments/ms3-traceability-matrix-group5-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zohrab Zeynalli\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zohrab Zeynalli\OneDrive\Documents\SENECA\2semester\SFT221\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8A1D73-B3B7-4567-9540-44DE560C661A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A1C097-7A4F-4B3A-A750-2DEE081C1685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1692" yWindow="36" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Actual Results</t>
   </si>
   <si>
-    <t>Pass / Fail</t>
-  </si>
-  <si>
     <t>R001</t>
   </si>
   <si>
@@ -425,6 +422,9 @@
   </si>
   <si>
     <t>Error handling and acceptance of correct input</t>
+  </si>
+  <si>
+    <t>Pass OR Fail</t>
   </si>
 </sst>
 </file>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -891,29 +891,29 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="43.2" customHeight="1">
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
@@ -937,7 +937,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
@@ -950,7 +950,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
@@ -967,13 +967,13 @@
     </row>
     <row r="8" spans="1:13" ht="43.2" customHeight="1">
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2">
         <v>0.25</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
@@ -997,7 +997,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
@@ -1053,16 +1053,16 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="2" t="b">
         <v>1</v>
@@ -1070,12 +1070,12 @@
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="b">
         <v>1</v>
@@ -1083,12 +1083,12 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="2" t="b">
         <v>0</v>
@@ -1096,12 +1096,12 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="2" t="b">
         <v>0</v>
@@ -1109,12 +1109,12 @@
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="2" t="b">
         <v>0</v>
@@ -1122,12 +1122,12 @@
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="2" t="b">
         <v>0</v>
@@ -1135,12 +1135,12 @@
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2" t="b">
         <v>1</v>
@@ -1148,12 +1148,12 @@
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="2" t="b">
         <v>0</v>
@@ -1161,12 +1161,12 @@
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="2" t="b">
         <v>0</v>
@@ -1174,12 +1174,12 @@
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="2" t="b">
         <v>0</v>
@@ -1190,136 +1190,136 @@
     </row>
     <row r="26" spans="2:6" ht="28.8" customHeight="1">
       <c r="B26" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="12"/>
       <c r="E27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="12"/>
       <c r="E28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="12"/>
       <c r="E29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="12"/>
       <c r="E30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="12"/>
       <c r="E31" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
       <c r="E32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
       <c r="E33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="12"/>
       <c r="E34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="12"/>
       <c r="E35" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>